<commit_message>
Minor changes to TestNG Asserts and Excel Utility
</commit_message>
<xml_diff>
--- a/TestData/EndPoint_Bus/GetBus_TestData.xlsx
+++ b/TestData/EndPoint_Bus/GetBus_TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>source</t>
   </si>
@@ -48,6 +48,27 @@
   </si>
   <si>
     <t>json</t>
+  </si>
+  <si>
+    <t>expectedcount</t>
+  </si>
+  <si>
+    <t>20170603</t>
+  </si>
+  <si>
+    <t>hyderabad</t>
+  </si>
+  <si>
+    <t>goa</t>
+  </si>
+  <si>
+    <t>20170608</t>
+  </si>
+  <si>
+    <t>20170610</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -366,21 +387,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -396,8 +418,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -407,31 +432,60 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
-        <v>20170604</v>
-      </c>
-      <c r="E2" s="1">
-        <v>20170608</v>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
-        <v>20170604</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
         <v>20170608</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2 D3:E4 D2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>